<commit_message>
add : test read txt table
</commit_message>
<xml_diff>
--- a/database/data/Species.xlsx
+++ b/database/data/Species.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New Course\PBL2\PBL2\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8AFCBC-CEB0-450B-BED0-259660DA3D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60758FA-4923-4F21-BC1A-6338E90EA75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -270,12 +270,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,21 +558,21 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
@@ -592,7 +591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -612,7 +611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -632,7 +631,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -652,7 +651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -672,7 +671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -692,7 +691,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -712,7 +711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -732,7 +731,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -752,7 +751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -772,7 +771,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -792,7 +791,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -812,7 +811,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -832,7 +831,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -852,7 +851,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>66</v>
       </c>

</xml_diff>